<commit_message>
R22 - Player Repeat Hit
Player can hit repeatedly test passes
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2BAF31-2458-4D57-B7A5-CFD68DB99147}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C696F1A8-9947-4843-A0F2-B5075DF31939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21">
@@ -1170,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22">

</xml_diff>

<commit_message>
R24, R25, Not Done, Done, Respectively
R24 is not done and I'll leave it for later. R25 is done (player busts and dealer wins because of it)
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F7A585-C160-4EAF-8D4B-5FA24858064C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6881B0C2-62B7-46EC-BF2F-AD88DFB9DF2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -864,7 +864,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25">

</xml_diff>

<commit_message>
R26, R27 Tests Done
Tests for R26 and R27 done. Dealer hits when its score is 16 or under and when it has a soft 17
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6881B0C2-62B7-46EC-BF2F-AD88DFB9DF2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576D18E3-706C-4F24-ADD0-5723B2D8E4F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1254,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26">
@@ -1275,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27">

</xml_diff>

<commit_message>
R31 and R32 Done
Tests for Aces counting as 1 or 11 are completed
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C27D98-017A-439F-8FFD-754942EFE8C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B77ADF2-6286-44C0-BEE5-425005BE6406}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1359,7 +1359,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31">
@@ -1380,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32">

</xml_diff>

<commit_message>
R44 and R45 Done
If there are no busts, player with highest score wins. If dealer and player have the same score, dealer wins. Both tests pass
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25863B14-BAC2-45F2-8505-2EEC7345FC00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FFF49F-00A1-415E-8D28-7E5593A72AFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
   <si>
     <t>Your game starts</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Pardo Antigua</t>
   </si>
 </sst>
 </file>
@@ -863,14 +869,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.796875" style="4"/>
+    <col min="5" max="5" width="13.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -880,15 +887,21 @@
       <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2">
+        <v>100948836</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -938,7 +951,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6">
@@ -1623,7 +1636,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44">
@@ -1644,7 +1657,7 @@
         <v>18</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45">

</xml_diff>

<commit_message>
R47 - Test Player Split
Starting writing a test for player split support. Neither the test nor the code are done
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Documents\School\University\Present_Classes\COMP_3004\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E459E9FD-9D52-48EA-8F2E-D5B00935FCD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F72544-F0FF-436F-99A8-67DB90C69853}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11040" windowHeight="3084" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="85">
   <si>
     <t>Your game starts</t>
   </si>
@@ -877,7 +877,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A31" sqref="A31:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1375,7 +1375,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1396,7 +1396,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1417,7 +1417,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1438,7 +1438,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1459,7 +1459,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="2" t="s">

</xml_diff>